<commit_message>
Less noises on the output image
Filter out 80% reflections from the road. Better quality.
</commit_message>
<xml_diff>
--- a/AMI_Project/data/record_data.xlsx
+++ b/AMI_Project/data/record_data.xlsx
@@ -1041,7 +1041,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:B1048576"/>
@@ -1051,650 +1051,154 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-8.309913635253906</v>
+        <v>-8.309860229492188</v>
       </c>
       <c r="B1" t="n">
-        <v>25.91148567199707</v>
+        <v>25.91147804260254</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-8.309913635253906</v>
+        <v>-8.309860229492188</v>
       </c>
       <c r="B2" t="n">
-        <v>25.91148567199707</v>
+        <v>25.91147804260254</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-7.812427997589111</v>
+        <v>-7.923340797424316</v>
       </c>
       <c r="B3" t="n">
-        <v>27.90762901306152</v>
+        <v>27.88959503173828</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-7.240021228790283</v>
+        <v>-7.506770610809326</v>
       </c>
       <c r="B4" t="n">
-        <v>29.82939338684082</v>
+        <v>30.1965274810791</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-6.515647411346436</v>
+        <v>-7.200259208679199</v>
       </c>
       <c r="B5" t="n">
-        <v>31.84791374206543</v>
+        <v>32.2003288269043</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-5.371394634246826</v>
+        <v>-6.954334735870361</v>
       </c>
       <c r="B6" t="n">
-        <v>33.70674896240234</v>
+        <v>34.19545745849609</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-3.389470338821411</v>
+        <v>-6.746068477630615</v>
       </c>
       <c r="B7" t="n">
-        <v>34.42194366455078</v>
+        <v>36.48851013183594</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-1.552290797233582</v>
+        <v>-6.617000579833984</v>
       </c>
       <c r="B8" t="n">
-        <v>33.58741760253906</v>
+        <v>38.66115570068359</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.004481944721192122</v>
+        <v>-6.540402889251709</v>
       </c>
       <c r="B9" t="n">
-        <v>32.21493911743164</v>
+        <v>40.83989334106445</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1.41100537776947</v>
+        <v>-6.50297212600708</v>
       </c>
       <c r="B10" t="n">
-        <v>30.79125022888184</v>
+        <v>42.98240280151367</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>3.014750003814697</v>
+        <v>-6.492049217224121</v>
       </c>
       <c r="B11" t="n">
-        <v>29.58205032348633</v>
+        <v>45.23105239868164</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>4.463268280029297</v>
+        <v>-6.50359058380127</v>
       </c>
       <c r="B12" t="n">
-        <v>28.19297218322754</v>
+        <v>47.43316268920898</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>5.803157806396484</v>
+        <v>-6.53030252456665</v>
       </c>
       <c r="B13" t="n">
-        <v>26.55780220031738</v>
+        <v>49.46305084228516</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>7.059130668640137</v>
+        <v>-6.565435409545898</v>
       </c>
       <c r="B14" t="n">
-        <v>24.97375106811523</v>
+        <v>51.55378341674805</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>8.30673885345459</v>
+        <v>-6.597684860229492</v>
       </c>
       <c r="B15" t="n">
-        <v>23.35039901733398</v>
+        <v>53.56374740600586</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>9.641523361206055</v>
+        <v>-6.620381832122803</v>
       </c>
       <c r="B16" t="n">
-        <v>21.63960838317871</v>
+        <v>55.65523147583008</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>11.07501029968262</v>
+        <v>-6.629554748535156</v>
       </c>
       <c r="B17" t="n">
-        <v>19.97068405151367</v>
+        <v>57.67204284667969</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>12.61462211608887</v>
+        <v>-6.626868724822998</v>
       </c>
       <c r="B18" t="n">
-        <v>18.35730934143066</v>
+        <v>59.97574234008789</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>14.14200210571289</v>
+        <v>-6.616115093231201</v>
       </c>
       <c r="B19" t="n">
-        <v>16.76203346252441</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>15.43952369689941</v>
-      </c>
-      <c r="B20" t="n">
-        <v>15.19657707214355</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>16.63017654418945</v>
-      </c>
-      <c r="B21" t="n">
-        <v>13.50136661529541</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>17.7419548034668</v>
-      </c>
-      <c r="B22" t="n">
-        <v>11.60062026977539</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>18.65431785583496</v>
-      </c>
-      <c r="B23" t="n">
-        <v>9.639179229736328</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>19.29173851013184</v>
-      </c>
-      <c r="B24" t="n">
-        <v>7.740952491760254</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>19.69988250732422</v>
-      </c>
-      <c r="B25" t="n">
-        <v>5.73197603225708</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>19.85392379760742</v>
-      </c>
-      <c r="B26" t="n">
-        <v>3.645110368728638</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>19.73513412475586</v>
-      </c>
-      <c r="B27" t="n">
-        <v>1.511914849281311</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>19.36038208007812</v>
-      </c>
-      <c r="B28" t="n">
-        <v>-0.5290524959564209</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>18.79901123046875</v>
-      </c>
-      <c r="B29" t="n">
-        <v>-2.542325496673584</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>18.21873474121094</v>
-      </c>
-      <c r="B30" t="n">
-        <v>-4.510073184967041</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>17.51382446289062</v>
-      </c>
-      <c r="B31" t="n">
-        <v>-6.489689350128174</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>16.64222526550293</v>
-      </c>
-      <c r="B32" t="n">
-        <v>-8.361025810241699</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>15.59588146209717</v>
-      </c>
-      <c r="B33" t="n">
-        <v>-10.14261150360107</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>14.40043830871582</v>
-      </c>
-      <c r="B34" t="n">
-        <v>-11.79730415344238</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>13.01813411712646</v>
-      </c>
-      <c r="B35" t="n">
-        <v>-13.37093257904053</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>11.40670394897461</v>
-      </c>
-      <c r="B36" t="n">
-        <v>-14.87558841705322</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>9.648234367370605</v>
-      </c>
-      <c r="B37" t="n">
-        <v>-16.21146965026855</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>7.922410011291504</v>
-      </c>
-      <c r="B38" t="n">
-        <v>-17.27499771118164</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>6.062253475189209</v>
-      </c>
-      <c r="B39" t="n">
-        <v>-18.19206428527832</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>3.894786834716797</v>
-      </c>
-      <c r="B40" t="n">
-        <v>-19.00116729736328</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>1.776720404624939</v>
-      </c>
-      <c r="B41" t="n">
-        <v>-19.55084991455078</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>-0.2913518846035004</v>
-      </c>
-      <c r="B42" t="n">
-        <v>-19.87533569335938</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>-2.565606594085693</v>
-      </c>
-      <c r="B43" t="n">
-        <v>-20.00134658813477</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>-4.574290752410889</v>
-      </c>
-      <c r="B44" t="n">
-        <v>-19.91488456726074</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>-6.591915130615234</v>
-      </c>
-      <c r="B45" t="n">
-        <v>-19.63919067382812</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>-8.730314254760742</v>
-      </c>
-      <c r="B46" t="n">
-        <v>-19.13206100463867</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>-10.64982032775879</v>
-      </c>
-      <c r="B47" t="n">
-        <v>-18.47515678405762</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>-12.70480918884277</v>
-      </c>
-      <c r="B48" t="n">
-        <v>-17.53772163391113</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>-14.66769123077393</v>
-      </c>
-      <c r="B49" t="n">
-        <v>-16.38251495361328</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>-16.47997856140137</v>
-      </c>
-      <c r="B50" t="n">
-        <v>-15.04522895812988</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>-18.01966857910156</v>
-      </c>
-      <c r="B51" t="n">
-        <v>-13.6540412902832</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>-19.38949012756348</v>
-      </c>
-      <c r="B52" t="n">
-        <v>-12.16000938415527</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>-20.72894287109375</v>
-      </c>
-      <c r="B53" t="n">
-        <v>-10.3782320022583</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>-21.88462066650391</v>
-      </c>
-      <c r="B54" t="n">
-        <v>-8.460554122924805</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>-22.84261512756348</v>
-      </c>
-      <c r="B55" t="n">
-        <v>-6.423665523529053</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>-23.58078384399414</v>
-      </c>
-      <c r="B56" t="n">
-        <v>-4.316716194152832</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>-24.11890602111816</v>
-      </c>
-      <c r="B57" t="n">
-        <v>-2.044051885604858</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>-24.41135215759277</v>
-      </c>
-      <c r="B58" t="n">
-        <v>0.2711431384086609</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>-24.46308135986328</v>
-      </c>
-      <c r="B59" t="n">
-        <v>2.335273742675781</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>-24.32091903686523</v>
-      </c>
-      <c r="B60" t="n">
-        <v>4.386609554290771</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>-23.97048759460449</v>
-      </c>
-      <c r="B61" t="n">
-        <v>6.490757942199707</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>-23.42817115783691</v>
-      </c>
-      <c r="B62" t="n">
-        <v>8.515415191650391</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>-22.66974830627441</v>
-      </c>
-      <c r="B63" t="n">
-        <v>10.53631687164307</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>-21.04305076599121</v>
-      </c>
-      <c r="B64" t="n">
-        <v>13.60267066955566</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>-19.72568702697754</v>
-      </c>
-      <c r="B65" t="n">
-        <v>15.52070426940918</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>-18.71841239929199</v>
-      </c>
-      <c r="B66" t="n">
-        <v>17.36954689025879</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>-18.29244804382324</v>
-      </c>
-      <c r="B67" t="n">
-        <v>19.54180908203125</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>-18.1338062286377</v>
-      </c>
-      <c r="B68" t="n">
-        <v>21.60541725158691</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>-18.20076370239258</v>
-      </c>
-      <c r="B69" t="n">
-        <v>23.63907623291016</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>-18.56122207641602</v>
-      </c>
-      <c r="B70" t="n">
-        <v>25.86523056030273</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>-18.71603202819824</v>
-      </c>
-      <c r="B71" t="n">
-        <v>28.15022850036621</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>-18.59053611755371</v>
-      </c>
-      <c r="B72" t="n">
-        <v>30.25747680664062</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>-18.62489891052246</v>
-      </c>
-      <c r="B73" t="n">
-        <v>32.3758659362793</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>-18.79111671447754</v>
-      </c>
-      <c r="B74" t="n">
-        <v>34.65810394287109</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>-18.78403282165527</v>
-      </c>
-      <c r="B75" t="n">
-        <v>36.70377731323242</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>-18.5408763885498</v>
-      </c>
-      <c r="B76" t="n">
-        <v>41.16885757446289</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>-18.35637092590332</v>
-      </c>
-      <c r="B77" t="n">
-        <v>43.42361831665039</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>-18.12678909301758</v>
-      </c>
-      <c r="B78" t="n">
-        <v>45.70132064819336</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>-17.85740280151367</v>
-      </c>
-      <c r="B79" t="n">
-        <v>47.96929931640625</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>-17.56929588317871</v>
-      </c>
-      <c r="B80" t="n">
-        <v>50.07987213134766</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>-17.26665115356445</v>
-      </c>
-      <c r="B81" t="n">
-        <v>52.05922317504883</v>
+        <v>61.9943962097168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small changes are made for users of carla 0.9.12
../carla/dist/carla-*%d.%d-%s.egg
</commit_message>
<xml_diff>
--- a/AMI_Project/data/record_data.xlsx
+++ b/AMI_Project/data/record_data.xlsx
@@ -1041,7 +1041,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:B1048576"/>
@@ -1051,154 +1051,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-8.309860229492188</v>
+        <v>-8.309648513793945</v>
       </c>
       <c r="B1" t="n">
-        <v>25.91147804260254</v>
+        <v>25.9113883972168</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-8.309860229492188</v>
+        <v>-8.309648513793945</v>
       </c>
       <c r="B2" t="n">
-        <v>25.91147804260254</v>
+        <v>25.9113883972168</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-7.923340797424316</v>
+        <v>-7.909624576568604</v>
       </c>
       <c r="B3" t="n">
-        <v>27.88959503173828</v>
+        <v>27.96125221252441</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-7.506770610809326</v>
+        <v>-7.548133373260498</v>
       </c>
       <c r="B4" t="n">
-        <v>30.1965274810791</v>
+        <v>29.9398136138916</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-7.200259208679199</v>
+        <v>-7.231334209442139</v>
       </c>
       <c r="B5" t="n">
-        <v>32.2003288269043</v>
+        <v>31.95211791992188</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-6.954334735870361</v>
+        <v>-6.954930782318115</v>
       </c>
       <c r="B6" t="n">
-        <v>34.19545745849609</v>
+        <v>34.16864395141602</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-6.746068477630615</v>
+        <v>-6.753246784210205</v>
       </c>
       <c r="B7" t="n">
-        <v>36.48851013183594</v>
+        <v>36.38595581054688</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-6.617000579833984</v>
+        <v>-6.617630481719971</v>
       </c>
       <c r="B8" t="n">
-        <v>38.66115570068359</v>
+        <v>38.65129470825195</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-6.540402889251709</v>
+        <v>-6.54407262802124</v>
       </c>
       <c r="B9" t="n">
-        <v>40.83989334106445</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>-6.50297212600708</v>
-      </c>
-      <c r="B10" t="n">
-        <v>42.98240280151367</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>-6.492049217224121</v>
-      </c>
-      <c r="B11" t="n">
-        <v>45.23105239868164</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>-6.50359058380127</v>
-      </c>
-      <c r="B12" t="n">
-        <v>47.43316268920898</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>-6.53030252456665</v>
-      </c>
-      <c r="B13" t="n">
-        <v>49.46305084228516</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>-6.565435409545898</v>
-      </c>
-      <c r="B14" t="n">
-        <v>51.55378341674805</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>-6.597684860229492</v>
-      </c>
-      <c r="B15" t="n">
-        <v>53.56374740600586</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>-6.620381832122803</v>
-      </c>
-      <c r="B16" t="n">
-        <v>55.65523147583008</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>-6.629554748535156</v>
-      </c>
-      <c r="B17" t="n">
-        <v>57.67204284667969</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>-6.626868724822998</v>
-      </c>
-      <c r="B18" t="n">
-        <v>59.97574234008789</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>-6.616115093231201</v>
-      </c>
-      <c r="B19" t="n">
-        <v>61.9943962097168</v>
+        <v>40.74065399169922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>